<commit_message>
modify mold file format
</commit_message>
<xml_diff>
--- a/python/mutual_mold/files/06. PT. KBI.xlsx
+++ b/python/mutual_mold/files/06. PT. KBI.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01. RIZKA\1. ERP\DATA MOLDING\0_+-¿p¦MÑU+O«¦\MoldData_20231122\06. PT. KBI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED773701-CB4F-4D13-97AF-D3FF2EC39ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LIST MOLD" sheetId="1" r:id="rId1"/>
@@ -18,22 +12,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'LIST MOLD'!$A$1:$Q$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'LIST MOLD (2)'!$A$1:$R$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'LIST MOLD (2)'!$A$1:$Q$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -190,36 +171,46 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;NT$&quot;* #,##0.00_-;\-&quot;NT$&quot;* #,##0.00_-;_-&quot;NT$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;NT$&quot;* #,##0_-;\-&quot;NT$&quot;* #,##0_-;_-&quot;NT$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="30">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Trebuchet MS"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Trebuchet MS"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <name val="Trebuchet MS"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
+      <sz val="10"/>
+      <name val="Trebuchet MS"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -229,30 +220,366 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Tahoma"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -446,19 +773,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="double">
         <color auto="1"/>
@@ -542,389 +856,593 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="49" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="49" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="51">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 9" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Style 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal 9" xfId="49"/>
+    <cellStyle name="Style 1" xfId="50"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -935,7 +1453,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -963,47 +1481,161 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1019,32 +1651,20 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1134">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Group 1134"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="85725" y="47625"/>
-          <a:ext cx="2003903" cy="721551"/>
+          <a:ext cx="2009775" cy="733425"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="2162825" cy="773091"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
+      <xdr:sp>
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="WordArt 69">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
+          <xdr:cNvPr id="3" name="WordArt 69"/>
           <xdr:cNvSpPr>
             <a:spLocks noTextEdit="1"/>
           </xdr:cNvSpPr>
@@ -1149,24 +1769,27 @@
               </a:rPr>
               <a:t>PT. YUJU INDONESIA</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" sz="3600">
+              <a:solidFill>
+                <a:srgbClr val="333399">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" charset="0"/>
+              <a:ea typeface="Arial Black" panose="020B0A04020102020204" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 360">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
+          <xdr:cNvPr id="4" name="Picture 360"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip r:embed="rId1"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1192,7 +1815,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1201,39 +1824,27 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>243548</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1134">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Group 1134"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="150965" y="47625"/>
-          <a:ext cx="3106658" cy="759651"/>
+          <a:off x="150495" y="47625"/>
+          <a:ext cx="3255010" cy="771525"/>
           <a:chOff x="42305" y="0"/>
           <a:chExt cx="2014507" cy="773091"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
+      <xdr:sp>
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="WordArt 69">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
+          <xdr:cNvPr id="3" name="WordArt 69"/>
           <xdr:cNvSpPr>
             <a:spLocks noTextEdit="1"/>
           </xdr:cNvSpPr>
@@ -1338,24 +1949,27 @@
               </a:rPr>
               <a:t>PT. YUJU INDONESIA</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" sz="3600">
+              <a:solidFill>
+                <a:srgbClr val="333399">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" charset="0"/>
+              <a:ea typeface="Arial Black" panose="020B0A04020102020204" charset="0"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 360">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
+          <xdr:cNvPr id="4" name="Picture 360"/>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
         </xdr:nvPicPr>
         <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:blip r:embed="rId1"/>
           <a:stretch>
             <a:fillRect/>
           </a:stretch>
@@ -1632,15 +2246,15 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="73" zoomScaleNormal="85" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
@@ -1662,455 +2276,466 @@
     <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="58" t="s">
+    <row r="1" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="22" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="30"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="69"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="22" t="s">
+    <row r="2" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="22" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="30"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="69"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="22" t="s">
+    <row r="3" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="N3" s="22" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="30"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="69"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="22" t="s">
+    <row r="4" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="23"/>
-      <c r="N4" s="22" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="30"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="69"/>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A5" s="32" t="s">
+    <row r="5" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="67" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="54" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="71" t="s">
+      <c r="J5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="72"/>
-      <c r="L5" s="32" t="s">
+      <c r="K5" s="55"/>
+      <c r="L5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
       <c r="O5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="71" t="s">
+      <c r="P5" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="72"/>
+      <c r="Q5" s="55"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="13" t="s">
+    <row r="6" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="57"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="74"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="58"/>
     </row>
-    <row r="7" spans="1:17" ht="130.5" customHeight="1">
-      <c r="A7" s="14">
+    <row r="7" ht="130.5" customHeight="1" spans="1:17">
+      <c r="A7" s="30">
         <v>1</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="25">
+      <c r="C7" s="76"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36">
         <v>640</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="60">
         <v>2</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="16">
+      <c r="K7" s="62"/>
+      <c r="L7" s="35">
         <v>600</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="35">
         <v>510</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="35">
         <v>450</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="35">
         <v>805</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="39"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="70"/>
     </row>
-    <row r="8" spans="1:17" ht="132.75" customHeight="1">
-      <c r="A8" s="17">
+    <row r="8" ht="132.75" customHeight="1" spans="1:17">
+      <c r="A8" s="37">
         <f>+A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42" t="s">
+      <c r="C8" s="78"/>
+      <c r="D8" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="27" t="s">
+      <c r="E8" s="41"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="63">
         <v>2</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="45"/>
-      <c r="L8" s="17">
+      <c r="K8" s="65"/>
+      <c r="L8" s="37">
         <v>920</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="37">
         <v>420</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="37">
         <v>350</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="37">
         <v>791</v>
       </c>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="47"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="71"/>
     </row>
-    <row r="9" spans="1:17" ht="128.25" customHeight="1">
-      <c r="A9" s="31" t="s">
+    <row r="9" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A9" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="C9" s="79"/>
+      <c r="D9" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="49"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="27" t="s">
+      <c r="E9" s="44"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="63">
         <v>2</v>
       </c>
-      <c r="J9" s="50" t="s">
+      <c r="J9" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="50"/>
-      <c r="L9" s="17">
+      <c r="K9" s="66"/>
+      <c r="L9" s="37">
         <v>840</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="37">
         <v>450</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="37">
         <v>420</v>
       </c>
-      <c r="O9" s="17"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="52"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="72"/>
     </row>
-    <row r="10" spans="1:17" ht="128.25" customHeight="1">
-      <c r="A10" s="31" t="s">
+    <row r="10" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A10" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="79"/>
+      <c r="D10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="27" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="63">
         <v>1</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="50"/>
-      <c r="L10" s="17">
+      <c r="K10" s="66"/>
+      <c r="L10" s="37">
         <v>800</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="37">
         <v>750</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="37">
         <v>700</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="37">
         <v>2457</v>
       </c>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="52"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="72"/>
     </row>
-    <row r="11" spans="1:17" ht="128.25" customHeight="1">
-      <c r="A11" s="31" t="s">
+    <row r="11" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="79"/>
+      <c r="D11" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="49"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="27" t="s">
+      <c r="E11" s="44"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="63">
         <v>1</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="50"/>
-      <c r="L11" s="17">
+      <c r="K11" s="66"/>
+      <c r="L11" s="37">
         <v>800</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="37">
         <v>750</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11" s="37">
         <v>700</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="37">
         <v>2457</v>
       </c>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="52"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="72"/>
     </row>
-    <row r="12" spans="1:17" ht="128.25" customHeight="1">
-      <c r="A12" s="31" t="s">
+    <row r="12" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A12" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49" t="s">
+      <c r="C12" s="79"/>
+      <c r="D12" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="49"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="27" t="s">
+      <c r="E12" s="44"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="50" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="50"/>
-      <c r="L12" s="17">
+      <c r="K12" s="66"/>
+      <c r="L12" s="37">
         <v>800</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="37">
         <v>750</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="37">
         <v>700</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="37">
         <v>2457</v>
       </c>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="52"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="72"/>
     </row>
-    <row r="13" spans="1:17" ht="128.25" customHeight="1">
-      <c r="A13" s="31" t="s">
+    <row r="13" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A13" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49" t="s">
+      <c r="C13" s="79"/>
+      <c r="D13" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="49"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="27" t="s">
+      <c r="E13" s="44"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="50" t="s">
+      <c r="I13" s="63"/>
+      <c r="J13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="50"/>
-      <c r="L13" s="17">
+      <c r="K13" s="66"/>
+      <c r="L13" s="37">
         <v>800</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="37">
         <v>750</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="37">
         <v>700</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="37">
         <v>2457</v>
       </c>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="52"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="72"/>
     </row>
-    <row r="14" spans="1:17" ht="26.1" customHeight="1">
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="19"/>
+    <row r="14" ht="26.1" customHeight="1" spans="5:8">
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="45"/>
     </row>
-    <row r="15" spans="1:17" ht="26.1" customHeight="1"/>
-    <row r="16" spans="1:17" ht="98.1" customHeight="1">
-      <c r="K16" s="29"/>
+    <row r="15" ht="26.1" customHeight="1"/>
+    <row r="16" ht="98.1" customHeight="1" spans="11:11">
+      <c r="K16" s="68"/>
     </row>
     <row r="17" ht="98.1" customHeight="1"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E1:K4"/>
-    <mergeCell ref="B5:C6"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="P5:Q6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="P11:Q11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="J12:K12"/>
@@ -2119,588 +2744,557 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="O5:O6"/>
+    <mergeCell ref="E1:K4"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="P5:Q6"/>
   </mergeCells>
-  <pageMargins left="0.31458333333333299" right="0" top="0.27500000000000002" bottom="0.39305555555555599" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="89" fitToHeight="8" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.314583333333333" right="0" top="0.275" bottom="0.393055555555556" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="89" fitToHeight="8" orientation="landscape"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="10" max="16" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="73" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P1" sqref="P$1:Q$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="4.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.75" style="1" customWidth="1"/>
-    <col min="11" max="16" width="6.25" style="1" customWidth="1"/>
-    <col min="17" max="17" width="4.125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="3.375" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="18.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.75" style="1" customWidth="1"/>
+    <col min="10" max="15" width="6.25" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="7.375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.375" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="58" t="s">
+    <row r="1" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="22" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="22" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="30"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="69"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="22" t="s">
+    <row r="2" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="22" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="30"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="69"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="22" t="s">
+    <row r="3" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="23"/>
-      <c r="O3" s="22" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="30"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="69"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="22" t="s">
+    <row r="4" ht="15.75" customHeight="1" spans="1:17">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="23"/>
-      <c r="O4" s="22" t="s">
+      <c r="M4" s="50"/>
+      <c r="N4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="30"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="69"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" customHeight="1">
-      <c r="A5" s="32" t="s">
+    <row r="5" ht="18.75" customHeight="1" spans="1:17">
+      <c r="A5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="67" t="s">
+      <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="67" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="68"/>
-      <c r="G5" s="54" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="54" t="s">
+      <c r="G5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="H5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="I5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="71" t="s">
+      <c r="J5" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="72"/>
-      <c r="M5" s="32" t="s">
+      <c r="K5" s="55"/>
+      <c r="L5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="56" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="71" t="s">
+      <c r="P5" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="72"/>
+      <c r="Q5" s="55"/>
     </row>
-    <row r="6" spans="1:18" ht="27.95" customHeight="1">
-      <c r="A6" s="53"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="13" t="s">
+    <row r="6" ht="27.95" customHeight="1" spans="1:17">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="M6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="N6" s="25" t="s">
         <v>22</v>
       </c>
+      <c r="O6" s="59"/>
       <c r="P6" s="57"/>
-      <c r="Q6" s="73"/>
-      <c r="R6" s="74"/>
+      <c r="Q6" s="58"/>
     </row>
-    <row r="7" spans="1:18" ht="130.5" customHeight="1">
-      <c r="A7" s="14">
+    <row r="7" ht="130.5" customHeight="1" spans="1:17">
+      <c r="A7" s="30">
         <v>1</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35" t="s">
+      <c r="D7" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="25">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36">
         <v>640</v>
       </c>
-      <c r="J7" s="26">
+      <c r="I7" s="60">
         <v>2</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="J7" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="38"/>
-      <c r="M7" s="16">
+      <c r="K7" s="62"/>
+      <c r="L7" s="35">
         <v>600</v>
       </c>
-      <c r="N7" s="16">
+      <c r="M7" s="35">
         <v>510</v>
       </c>
-      <c r="O7" s="16">
+      <c r="N7" s="35">
         <v>450</v>
       </c>
-      <c r="P7" s="16">
+      <c r="O7" s="35">
         <v>805</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="39"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="70"/>
     </row>
-    <row r="8" spans="1:18" ht="132.75" customHeight="1">
-      <c r="A8" s="17">
+    <row r="8" ht="132.75" customHeight="1" spans="1:17">
+      <c r="A8" s="37">
         <f>+A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42" t="s">
+      <c r="D8" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="43"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="27" t="s">
+      <c r="E8" s="41"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="28">
+      <c r="I8" s="63">
         <v>2</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="J8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="45"/>
-      <c r="M8" s="17">
+      <c r="K8" s="65"/>
+      <c r="L8" s="37">
         <v>920</v>
       </c>
-      <c r="N8" s="17">
+      <c r="M8" s="37">
         <v>420</v>
       </c>
-      <c r="O8" s="17">
+      <c r="N8" s="37">
         <v>350</v>
       </c>
-      <c r="P8" s="17">
+      <c r="O8" s="37">
         <v>791</v>
       </c>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="47"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="71"/>
     </row>
-    <row r="9" spans="1:18" ht="128.25" customHeight="1">
-      <c r="A9" s="31" t="s">
+    <row r="9" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A9" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49" t="s">
+      <c r="D9" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="27" t="s">
+      <c r="E9" s="44"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="28">
+      <c r="I9" s="63">
         <v>2</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="J9" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="50"/>
-      <c r="M9" s="17">
+      <c r="K9" s="66"/>
+      <c r="L9" s="37">
         <v>840</v>
       </c>
-      <c r="N9" s="17">
+      <c r="M9" s="37">
         <v>450</v>
       </c>
-      <c r="O9" s="17">
+      <c r="N9" s="37">
         <v>420</v>
       </c>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="52"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="67"/>
+      <c r="Q9" s="72"/>
     </row>
-    <row r="10" spans="1:18" ht="128.25" customHeight="1">
-      <c r="A10" s="31" t="s">
+    <row r="10" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A10" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49" t="s">
+      <c r="D10" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="27" t="s">
+      <c r="E10" s="44"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="28">
+      <c r="I10" s="63">
         <v>1</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="J10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="50"/>
-      <c r="M10" s="17">
+      <c r="K10" s="66"/>
+      <c r="L10" s="37">
         <v>800</v>
       </c>
-      <c r="N10" s="17">
+      <c r="M10" s="37">
         <v>750</v>
       </c>
-      <c r="O10" s="17">
+      <c r="N10" s="37">
         <v>700</v>
       </c>
-      <c r="P10" s="17">
+      <c r="O10" s="37">
         <v>2457</v>
       </c>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="52"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="72"/>
     </row>
-    <row r="11" spans="1:18" ht="128.25" customHeight="1">
-      <c r="A11" s="31" t="s">
+    <row r="11" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A11" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49" t="s">
+      <c r="D11" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="27" t="s">
+      <c r="E11" s="44"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="28">
+      <c r="I11" s="63">
         <v>1</v>
       </c>
-      <c r="K11" s="50" t="s">
+      <c r="J11" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="50"/>
-      <c r="M11" s="17">
+      <c r="K11" s="66"/>
+      <c r="L11" s="37">
         <v>800</v>
       </c>
-      <c r="N11" s="17">
+      <c r="M11" s="37">
         <v>750</v>
       </c>
-      <c r="O11" s="17">
+      <c r="N11" s="37">
         <v>700</v>
       </c>
-      <c r="P11" s="17">
+      <c r="O11" s="37">
         <v>2457</v>
       </c>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="52"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="72"/>
     </row>
-    <row r="12" spans="1:18" ht="128.25" customHeight="1">
-      <c r="A12" s="31" t="s">
+    <row r="12" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A12" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49" t="s">
+      <c r="D12" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="27" t="s">
+      <c r="E12" s="44"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="50" t="s">
+      <c r="I12" s="63"/>
+      <c r="J12" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="50"/>
-      <c r="M12" s="17">
+      <c r="K12" s="66"/>
+      <c r="L12" s="37">
         <v>800</v>
       </c>
-      <c r="N12" s="17">
+      <c r="M12" s="37">
         <v>750</v>
       </c>
-      <c r="O12" s="17">
+      <c r="N12" s="37">
         <v>700</v>
       </c>
-      <c r="P12" s="17">
+      <c r="O12" s="37">
         <v>2457</v>
       </c>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="52"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="72"/>
     </row>
-    <row r="13" spans="1:18" ht="128.25" customHeight="1">
-      <c r="A13" s="31" t="s">
+    <row r="13" ht="128.25" customHeight="1" spans="1:17">
+      <c r="A13" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="49" t="s">
+      <c r="D13" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="27" t="s">
+      <c r="E13" s="44"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="28"/>
-      <c r="K13" s="50" t="s">
+      <c r="I13" s="63"/>
+      <c r="J13" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="50"/>
-      <c r="M13" s="17">
+      <c r="K13" s="66"/>
+      <c r="L13" s="37">
         <v>800</v>
       </c>
-      <c r="N13" s="17">
+      <c r="M13" s="37">
         <v>750</v>
       </c>
-      <c r="O13" s="17">
+      <c r="N13" s="37">
         <v>700</v>
       </c>
-      <c r="P13" s="17">
+      <c r="O13" s="37">
         <v>2457</v>
       </c>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="52"/>
+      <c r="P13" s="67"/>
+      <c r="Q13" s="72"/>
     </row>
-    <row r="14" spans="1:18" ht="26.1" customHeight="1">
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="19"/>
+    <row r="14" ht="26.1" customHeight="1" spans="5:8">
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="45"/>
     </row>
-    <row r="15" spans="1:18" ht="26.1" customHeight="1"/>
-    <row r="16" spans="1:18" ht="98.1" customHeight="1">
-      <c r="L16" s="29"/>
+    <row r="15" ht="26.1" customHeight="1"/>
+    <row r="16" ht="98.1" customHeight="1" spans="11:11">
+      <c r="K16" s="68"/>
     </row>
     <row r="17" ht="98.1" customHeight="1"/>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="F1:L4"/>
-    <mergeCell ref="C5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="Q5:R6"/>
+  <mergeCells count="34">
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="P13:Q13"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="E1:K4"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="P5:Q6"/>
   </mergeCells>
-  <pageMargins left="0.31458333333333299" right="0" top="0.27500000000000002" bottom="0.39305555555555599" header="0" footer="0"/>
-  <pageSetup paperSize="5" scale="89" fitToHeight="8" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.314583333333333" right="0" top="0.275" bottom="0.393055555555556" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="89" fitToHeight="8" orientation="landscape"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="10" max="17" man="1"/>
+    <brk id="10" max="16" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>